<commit_message>
scraping from second xlsx
</commit_message>
<xml_diff>
--- a/Carmax_CS_Hackathon_UseCasesFinal.xlsx
+++ b/Carmax_CS_Hackathon_UseCasesFinal.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuang/code/revenue-forecast-analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB8598-85A5-4D40-B8C5-0B3C046D3CFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="25035" windowHeight="14115"/>
+    <workbookView xWindow="16800" yWindow="440" windowWidth="16800" windowHeight="19380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit and Per Unit Metrics" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Unit and Per Unit Metrics'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="50">
   <si>
     <t>Retail Used Vehicles</t>
   </si>
@@ -172,7 +178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="0\ %;\ \(0\)%"/>
@@ -308,7 +314,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,9 +347,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,6 +399,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -551,30 +591,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
-    <col min="4" max="7" width="7.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="47.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="7.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -588,7 +628,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
@@ -603,12 +643,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
@@ -620,12 +660,12 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4">
-        <v>40387</v>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E6" s="4">
         <v>43119</v>
@@ -638,7 +678,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
@@ -656,7 +696,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
@@ -674,7 +714,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -692,7 +732,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -710,7 +750,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
@@ -728,7 +768,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
@@ -746,7 +786,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
@@ -764,7 +804,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
@@ -782,7 +822,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
@@ -800,7 +840,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
@@ -818,7 +858,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C17" s="1" t="s">
         <v>11</v>
       </c>
@@ -836,7 +876,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
@@ -854,7 +894,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
@@ -872,7 +912,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C20" s="1" t="s">
         <v>40</v>
       </c>
@@ -890,7 +930,7 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C21" s="1" t="s">
         <v>47</v>
       </c>
@@ -908,7 +948,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C22" s="1" t="s">
         <v>48</v>
       </c>
@@ -926,7 +966,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.15">
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -935,7 +975,7 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
@@ -947,7 +987,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C25" s="1" t="s">
         <v>16</v>
       </c>
@@ -965,13 +1005,13 @@
       <c r="I25" s="9"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="9" t="e">
         <f>D7/D6-1</f>
-        <v>0.17141654492782332</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E26" s="9">
         <f>E7/E6-1</f>
@@ -986,7 +1026,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1047,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1068,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1089,7 @@
       <c r="I29" s="9"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1110,7 @@
       <c r="I30" s="9"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1091,7 +1131,7 @@
       <c r="I31" s="9"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1152,7 @@
       <c r="I32" s="9"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1173,7 @@
       <c r="I33" s="9"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1194,7 @@
       <c r="I34" s="9"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
@@ -1175,7 +1215,7 @@
       <c r="I35" s="9"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1196,7 +1236,7 @@
       <c r="I36" s="9"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
@@ -1217,7 +1257,7 @@
       <c r="I37" s="9"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C38" s="1" t="s">
         <v>31</v>
       </c>
@@ -1238,7 +1278,7 @@
       <c r="I38" s="9"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C39" s="1" t="s">
         <v>40</v>
       </c>
@@ -1259,7 +1299,7 @@
       <c r="I39" s="9"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C40" s="1" t="s">
         <v>47</v>
       </c>
@@ -1280,7 +1320,7 @@
       <c r="I40" s="9"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C41" s="1" t="s">
         <v>48</v>
       </c>
@@ -1301,7 +1341,7 @@
       <c r="I41" s="9"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.15">
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1310,7 +1350,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>33</v>
       </c>
@@ -1322,7 +1362,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C44" s="1" t="s">
         <v>16</v>
       </c>
@@ -1340,7 +1380,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1398,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C46" s="1" t="s">
         <v>15</v>
       </c>
@@ -1376,7 +1416,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C47" s="1" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1434,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1452,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1430,7 +1470,7 @@
       <c r="I49" s="9"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C50" s="1" t="s">
         <v>14</v>
       </c>
@@ -1448,7 +1488,7 @@
       <c r="I50" s="9"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
@@ -1467,7 +1507,7 @@
       <c r="I51" s="9"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1485,7 +1525,7 @@
       <c r="I52" s="9"/>
       <c r="J52" s="4"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C53" s="1" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1543,7 @@
       <c r="I53" s="9"/>
       <c r="J53" s="4"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C54" s="1" t="s">
         <v>13</v>
       </c>
@@ -1521,7 +1561,7 @@
       <c r="I54" s="9"/>
       <c r="J54" s="4"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C55" s="1" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1579,7 @@
       <c r="I55" s="9"/>
       <c r="J55" s="4"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C56" s="1" t="s">
         <v>12</v>
       </c>
@@ -1557,7 +1597,7 @@
       <c r="I56" s="9"/>
       <c r="J56" s="4"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C57" s="1" t="s">
         <v>31</v>
       </c>
@@ -1575,7 +1615,7 @@
       <c r="I57" s="9"/>
       <c r="J57" s="4"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C58" s="1" t="s">
         <v>40</v>
       </c>
@@ -1593,7 +1633,7 @@
       <c r="I58" s="9"/>
       <c r="J58" s="4"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C59" s="1" t="s">
         <v>47</v>
       </c>
@@ -1611,7 +1651,7 @@
       <c r="I59" s="9"/>
       <c r="J59" s="4"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C60" s="1" t="s">
         <v>48</v>
       </c>
@@ -1630,7 +1670,7 @@
       <c r="I60" s="9"/>
       <c r="J60" s="4"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.15">
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -1639,7 +1679,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
@@ -1650,7 +1690,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C63" s="1" t="s">
         <v>16</v>
       </c>
@@ -1667,7 +1707,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +1724,7 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C65" s="1" t="s">
         <v>15</v>
       </c>
@@ -1701,7 +1741,7 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C66" s="1" t="s">
         <v>5</v>
       </c>
@@ -1718,7 +1758,7 @@
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C67" s="1" t="s">
         <v>6</v>
       </c>
@@ -1735,7 +1775,7 @@
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
@@ -1752,7 +1792,7 @@
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C69" s="1" t="s">
         <v>14</v>
       </c>
@@ -1769,7 +1809,7 @@
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C70" s="1" t="s">
         <v>8</v>
       </c>
@@ -1786,7 +1826,7 @@
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C71" s="1" t="s">
         <v>9</v>
       </c>
@@ -1803,7 +1843,7 @@
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C72" s="1" t="s">
         <v>10</v>
       </c>
@@ -1820,7 +1860,7 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C73" s="1" t="s">
         <v>13</v>
       </c>
@@ -1837,7 +1877,7 @@
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C74" s="1" t="s">
         <v>11</v>
       </c>
@@ -1854,7 +1894,7 @@
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C75" s="1" t="s">
         <v>12</v>
       </c>
@@ -1871,7 +1911,7 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C76" s="1" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1928,7 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C77" s="1" t="s">
         <v>40</v>
       </c>
@@ -1905,7 +1945,7 @@
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C78" s="1" t="s">
         <v>47</v>
       </c>
@@ -1922,7 +1962,7 @@
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:9" x14ac:dyDescent="0.15">
       <c r="C79" s="1" t="s">
         <v>48</v>
       </c>
@@ -1939,7 +1979,7 @@
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B81" s="1" t="s">
         <v>24</v>
       </c>
@@ -1950,7 +1990,7 @@
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
@@ -1967,7 +2007,7 @@
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C83" s="1" t="s">
         <v>15</v>
       </c>
@@ -1984,7 +2024,7 @@
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C84" s="1" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +2041,7 @@
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C85" s="1" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2058,7 @@
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
@@ -2035,7 +2075,7 @@
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C87" s="1" t="s">
         <v>14</v>
       </c>
@@ -2052,7 +2092,7 @@
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C88" s="1" t="s">
         <v>8</v>
       </c>
@@ -2069,7 +2109,7 @@
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C89" s="1" t="s">
         <v>9</v>
       </c>
@@ -2086,7 +2126,7 @@
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C90" s="1" t="s">
         <v>10</v>
       </c>
@@ -2103,7 +2143,7 @@
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C91" s="1" t="s">
         <v>13</v>
       </c>
@@ -2120,7 +2160,7 @@
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2177,7 @@
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C93" s="1" t="s">
         <v>12</v>
       </c>
@@ -2154,7 +2194,7 @@
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C94" s="1" t="s">
         <v>31</v>
       </c>
@@ -2171,7 +2211,7 @@
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C95" s="1" t="s">
         <v>40</v>
       </c>
@@ -2188,7 +2228,7 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C96" s="1" t="s">
         <v>47</v>
       </c>
@@ -2205,7 +2245,7 @@
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C97" s="1" t="s">
         <v>48</v>
       </c>
@@ -2222,12 +2262,12 @@
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A99" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B100" s="1" t="s">
         <v>22</v>
       </c>
@@ -2238,7 +2278,7 @@
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C101" s="1" t="s">
         <v>15</v>
       </c>
@@ -2255,7 +2295,7 @@
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C102" s="1" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +2312,7 @@
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C103" s="1" t="s">
         <v>6</v>
       </c>
@@ -2289,7 +2329,7 @@
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C104" s="1" t="s">
         <v>7</v>
       </c>
@@ -2306,7 +2346,7 @@
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C105" s="1" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2363,7 @@
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C106" s="1" t="s">
         <v>8</v>
       </c>
@@ -2340,7 +2380,7 @@
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C107" s="1" t="s">
         <v>9</v>
       </c>
@@ -2357,7 +2397,7 @@
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C108" s="1" t="s">
         <v>10</v>
       </c>
@@ -2374,7 +2414,7 @@
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C109" s="1" t="s">
         <v>13</v>
       </c>
@@ -2391,7 +2431,7 @@
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C110" s="1" t="s">
         <v>11</v>
       </c>
@@ -2408,7 +2448,7 @@
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C111" s="1" t="s">
         <v>12</v>
       </c>
@@ -2425,7 +2465,7 @@
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C112" s="1" t="s">
         <v>31</v>
       </c>
@@ -2442,7 +2482,7 @@
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C113" s="1" t="s">
         <v>40</v>
       </c>
@@ -2459,7 +2499,7 @@
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C114" s="1" t="s">
         <v>47</v>
       </c>
@@ -2476,7 +2516,7 @@
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C115" s="1" t="s">
         <v>48</v>
       </c>
@@ -2493,7 +2533,7 @@
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.15">
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -2501,7 +2541,7 @@
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B117" s="1" t="s">
         <v>37</v>
       </c>
@@ -2512,7 +2552,7 @@
       <c r="H117" s="8"/>
       <c r="I117" s="8"/>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C118" s="1" t="s">
         <v>5</v>
       </c>
@@ -2533,7 +2573,7 @@
       <c r="I118" s="9"/>
       <c r="J118" s="9"/>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C119" s="1" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2594,7 @@
       <c r="I119" s="9"/>
       <c r="J119" s="9"/>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C120" s="1" t="s">
         <v>7</v>
       </c>
@@ -2575,7 +2615,7 @@
       <c r="I120" s="9"/>
       <c r="J120" s="9"/>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C121" s="1" t="s">
         <v>14</v>
       </c>
@@ -2596,7 +2636,7 @@
       <c r="I121" s="9"/>
       <c r="J121" s="9"/>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C122" s="1" t="s">
         <v>8</v>
       </c>
@@ -2617,7 +2657,7 @@
       <c r="I122" s="9"/>
       <c r="J122" s="9"/>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C123" s="1" t="s">
         <v>9</v>
       </c>
@@ -2638,7 +2678,7 @@
       <c r="I123" s="9"/>
       <c r="J123" s="9"/>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C124" s="1" t="s">
         <v>10</v>
       </c>
@@ -2659,7 +2699,7 @@
       <c r="I124" s="9"/>
       <c r="J124" s="9"/>
     </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C125" s="1" t="s">
         <v>13</v>
       </c>
@@ -2680,7 +2720,7 @@
       <c r="I125" s="9"/>
       <c r="J125" s="9"/>
     </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C126" s="1" t="s">
         <v>11</v>
       </c>
@@ -2701,7 +2741,7 @@
       <c r="I126" s="9"/>
       <c r="J126" s="9"/>
     </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C127" s="1" t="s">
         <v>12</v>
       </c>
@@ -2721,7 +2761,7 @@
       <c r="H127" s="9"/>
       <c r="I127" s="9"/>
     </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C128" s="1" t="s">
         <v>31</v>
       </c>
@@ -2741,7 +2781,7 @@
       <c r="H128" s="9"/>
       <c r="I128" s="9"/>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C129" s="1" t="s">
         <v>40</v>
       </c>
@@ -2761,7 +2801,7 @@
       <c r="H129" s="9"/>
       <c r="I129" s="9"/>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C130" s="1" t="s">
         <v>47</v>
       </c>
@@ -2781,7 +2821,7 @@
       <c r="H130" s="9"/>
       <c r="I130" s="9"/>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C131" s="1" t="s">
         <v>48</v>
       </c>
@@ -2801,7 +2841,7 @@
       <c r="H131" s="9"/>
       <c r="I131" s="9"/>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.15">
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
@@ -2809,7 +2849,7 @@
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B133" s="1" t="s">
         <v>34</v>
       </c>
@@ -2820,7 +2860,7 @@
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C134" s="1" t="s">
         <v>5</v>
       </c>
@@ -2837,7 +2877,7 @@
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C135" s="1" t="s">
         <v>6</v>
       </c>
@@ -2854,7 +2894,7 @@
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C136" s="1" t="s">
         <v>7</v>
       </c>
@@ -2871,7 +2911,7 @@
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C137" s="1" t="s">
         <v>14</v>
       </c>
@@ -2888,7 +2928,7 @@
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C138" s="1" t="s">
         <v>8</v>
       </c>
@@ -2905,7 +2945,7 @@
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C139" s="1" t="s">
         <v>9</v>
       </c>
@@ -2922,7 +2962,7 @@
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C140" s="1" t="s">
         <v>10</v>
       </c>
@@ -2939,7 +2979,7 @@
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C141" s="1" t="s">
         <v>13</v>
       </c>
@@ -2956,7 +2996,7 @@
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C142" s="1" t="s">
         <v>11</v>
       </c>
@@ -2973,7 +3013,7 @@
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C143" s="1" t="s">
         <v>12</v>
       </c>
@@ -2990,7 +3030,7 @@
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C144" s="1" t="s">
         <v>31</v>
       </c>
@@ -3007,7 +3047,7 @@
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C145" s="1" t="s">
         <v>40</v>
       </c>
@@ -3024,7 +3064,7 @@
       <c r="H145" s="5"/>
       <c r="I145" s="5"/>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C146" s="1" t="s">
         <v>47</v>
       </c>
@@ -3041,7 +3081,7 @@
       <c r="H146" s="5"/>
       <c r="I146" s="5"/>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C147" s="1" t="s">
         <v>48</v>
       </c>
@@ -3058,7 +3098,7 @@
       <c r="H147" s="5"/>
       <c r="I147" s="5"/>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.15">
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
@@ -3066,7 +3106,7 @@
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B149" s="1" t="s">
         <v>23</v>
       </c>
@@ -3077,7 +3117,7 @@
       <c r="H149" s="5"/>
       <c r="I149" s="5"/>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C150" s="1" t="s">
         <v>15</v>
       </c>
@@ -3094,7 +3134,7 @@
       <c r="H150" s="5"/>
       <c r="I150" s="5"/>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C151" s="1" t="s">
         <v>5</v>
       </c>
@@ -3111,7 +3151,7 @@
       <c r="H151" s="5"/>
       <c r="I151" s="5"/>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C152" s="1" t="s">
         <v>6</v>
       </c>
@@ -3128,7 +3168,7 @@
       <c r="H152" s="5"/>
       <c r="I152" s="5"/>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C153" s="1" t="s">
         <v>7</v>
       </c>
@@ -3145,7 +3185,7 @@
       <c r="H153" s="5"/>
       <c r="I153" s="5"/>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C154" s="1" t="s">
         <v>14</v>
       </c>
@@ -3162,7 +3202,7 @@
       <c r="H154" s="5"/>
       <c r="I154" s="5"/>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C155" s="1" t="s">
         <v>8</v>
       </c>
@@ -3179,7 +3219,7 @@
       <c r="H155" s="5"/>
       <c r="I155" s="5"/>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C156" s="1" t="s">
         <v>9</v>
       </c>
@@ -3196,7 +3236,7 @@
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C157" s="1" t="s">
         <v>10</v>
       </c>
@@ -3213,7 +3253,7 @@
       <c r="H157" s="5"/>
       <c r="I157" s="5"/>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C158" s="1" t="s">
         <v>13</v>
       </c>
@@ -3230,7 +3270,7 @@
       <c r="H158" s="5"/>
       <c r="I158" s="5"/>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C159" s="1" t="s">
         <v>11</v>
       </c>
@@ -3247,7 +3287,7 @@
       <c r="H159" s="5"/>
       <c r="I159" s="5"/>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C160" s="1" t="s">
         <v>12</v>
       </c>
@@ -3264,7 +3304,7 @@
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C161" s="1" t="s">
         <v>31</v>
       </c>
@@ -3281,7 +3321,7 @@
       <c r="H161" s="5"/>
       <c r="I161" s="5"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C162" s="1" t="s">
         <v>40</v>
       </c>
@@ -3298,7 +3338,7 @@
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C163" s="1" t="s">
         <v>47</v>
       </c>
@@ -3315,7 +3355,7 @@
       <c r="H163" s="5"/>
       <c r="I163" s="5"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C164" s="1" t="s">
         <v>48</v>
       </c>
@@ -3332,17 +3372,17 @@
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A166" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B167" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C168" s="1" t="s">
         <v>15</v>
       </c>
@@ -3359,7 +3399,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C169" s="1" t="s">
         <v>5</v>
       </c>
@@ -3376,7 +3416,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="12"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C170" s="1" t="s">
         <v>6</v>
       </c>
@@ -3393,7 +3433,7 @@
       <c r="H170" s="12"/>
       <c r="I170" s="12"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C171" s="1" t="s">
         <v>7</v>
       </c>
@@ -3410,7 +3450,7 @@
       <c r="H171" s="12"/>
       <c r="I171" s="12"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C172" s="1" t="s">
         <v>14</v>
       </c>
@@ -3427,7 +3467,7 @@
       <c r="H172" s="12"/>
       <c r="I172" s="12"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C173" s="1" t="s">
         <v>8</v>
       </c>
@@ -3444,7 +3484,7 @@
       <c r="H173" s="12"/>
       <c r="I173" s="12"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C174" s="1" t="s">
         <v>9</v>
       </c>
@@ -3461,7 +3501,7 @@
       <c r="H174" s="12"/>
       <c r="I174" s="12"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C175" s="1" t="s">
         <v>10</v>
       </c>
@@ -3478,7 +3518,7 @@
       <c r="H175" s="12"/>
       <c r="I175" s="12"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C176" s="1" t="s">
         <v>13</v>
       </c>
@@ -3495,7 +3535,7 @@
       <c r="H176" s="12"/>
       <c r="I176" s="12"/>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C177" s="1" t="s">
         <v>11</v>
       </c>
@@ -3512,7 +3552,7 @@
       <c r="H177" s="12"/>
       <c r="I177" s="12"/>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C178" s="1" t="s">
         <v>12</v>
       </c>
@@ -3529,7 +3569,7 @@
       <c r="H178" s="12"/>
       <c r="I178" s="12"/>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C179" s="1" t="s">
         <v>31</v>
       </c>
@@ -3546,7 +3586,7 @@
       <c r="H179" s="12"/>
       <c r="I179" s="12"/>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C180" s="1" t="s">
         <v>40</v>
       </c>
@@ -3563,7 +3603,7 @@
       <c r="H180" s="12"/>
       <c r="I180" s="12"/>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C181" s="1" t="s">
         <v>47</v>
       </c>
@@ -3580,7 +3620,7 @@
       <c r="H181" s="12"/>
       <c r="I181" s="12"/>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C182" s="1" t="s">
         <v>48</v>
       </c>
@@ -3597,12 +3637,12 @@
       <c r="H182" s="12"/>
       <c r="I182" s="12"/>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B184" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C185" s="1" t="s">
         <v>9</v>
       </c>
@@ -3619,7 +3659,7 @@
       <c r="H185" s="10"/>
       <c r="I185" s="10"/>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C186" s="1" t="s">
         <v>10</v>
       </c>
@@ -3636,7 +3676,7 @@
       <c r="H186" s="11"/>
       <c r="I186" s="10"/>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C187" s="1" t="s">
         <v>13</v>
       </c>
@@ -3653,7 +3693,7 @@
       <c r="H187" s="11"/>
       <c r="I187" s="10"/>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C188" s="1" t="s">
         <v>11</v>
       </c>
@@ -3670,7 +3710,7 @@
       <c r="H188" s="11"/>
       <c r="I188" s="10"/>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C189" s="1" t="s">
         <v>12</v>
       </c>
@@ -3687,7 +3727,7 @@
       <c r="H189" s="11"/>
       <c r="I189" s="10"/>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C190" s="1" t="s">
         <v>31</v>
       </c>
@@ -3704,7 +3744,7 @@
       <c r="H190" s="11"/>
       <c r="I190" s="10"/>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C191" s="1" t="s">
         <v>40</v>
       </c>
@@ -3721,7 +3761,7 @@
       <c r="H191" s="10"/>
       <c r="I191" s="10"/>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C192" s="1" t="s">
         <v>47</v>
       </c>
@@ -3738,7 +3778,7 @@
       <c r="H192" s="10"/>
       <c r="I192" s="10"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C193" s="1" t="s">
         <v>48</v>
       </c>
@@ -3755,7 +3795,7 @@
       <c r="H193" s="10"/>
       <c r="I193" s="10"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.15">
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
       <c r="F194" s="11"/>
@@ -3763,7 +3803,7 @@
       <c r="H194" s="11"/>
       <c r="I194" s="11"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B196" s="7" t="s">
         <v>17</v>
       </c>
@@ -3771,7 +3811,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B197" s="7" t="s">
         <v>18</v>
       </c>
@@ -3779,13 +3819,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B198" s="7"/>
       <c r="C198" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B199" s="7" t="s">
         <v>27</v>
       </c>
@@ -3793,12 +3833,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C200" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
         <v>28</v>
       </c>
@@ -3806,12 +3846,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B207" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B208" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>